<commit_message>
Push team pix Create full.R file for cleaned up load/transform Fix summary file
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eab039813ee52d7e/Documents/R/ColumnHackathon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_FA361EC25B49EAD54E170B0BF31CC9A7502DDD3E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F2D368D-ABC7-44F1-AD41-0092D66105BB}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_FA361EC25B49EAD54E170B0BF31CC9A7502DDD3E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2922C716-8541-43B8-89E3-FF62E55484D7}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="4125" windowWidth="19020" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9375" yWindow="2880" windowWidth="19020" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="474">
   <si>
     <t>Duration</t>
   </si>
@@ -1453,9 +1453,6 @@
   </si>
   <si>
     <t>0:16:45.531</t>
-  </si>
-  <si>
-    <t>Open rate</t>
   </si>
 </sst>
 </file>
@@ -1987,11 +1984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L237"/>
+  <dimension ref="A1:J237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N206" sqref="N206:N213"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2002,7 @@
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -2036,11 +2033,8 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>191</v>
       </c>
@@ -2071,12 +2065,8 @@
       <c r="J2">
         <v>62</v>
       </c>
-      <c r="L2">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.38515351729498637</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>188</v>
       </c>
@@ -2107,12 +2097,8 @@
       <c r="J3">
         <v>54</v>
       </c>
-      <c r="L3">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.44366197183098594</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>234</v>
       </c>
@@ -2143,12 +2129,8 @@
       <c r="J4">
         <v>36</v>
       </c>
-      <c r="L4">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.47713884992987377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
@@ -2179,12 +2161,8 @@
       <c r="J5">
         <v>52</v>
       </c>
-      <c r="L5">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49414197105444518</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>151</v>
       </c>
@@ -2215,12 +2193,8 @@
       <c r="J6">
         <v>51</v>
       </c>
-      <c r="L6">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52464616886285997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2251,12 +2225,8 @@
       <c r="J7">
         <v>31</v>
       </c>
-      <c r="L7">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62728551336146277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>158</v>
       </c>
@@ -2287,12 +2257,8 @@
       <c r="J8">
         <v>61</v>
       </c>
-      <c r="L8">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52634054562558796</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>164</v>
       </c>
@@ -2323,12 +2289,8 @@
       <c r="J9">
         <v>59</v>
       </c>
-      <c r="L9">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48141745894554883</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>148</v>
       </c>
@@ -2359,12 +2321,8 @@
       <c r="J10">
         <v>52</v>
       </c>
-      <c r="L10">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.59118541033434646</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>189</v>
       </c>
@@ -2395,12 +2353,8 @@
       <c r="J11">
         <v>52</v>
       </c>
-      <c r="L11">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50824175824175821</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>186</v>
       </c>
@@ -2431,12 +2385,8 @@
       <c r="J12">
         <v>58</v>
       </c>
-      <c r="L12">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.40243902439024393</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>136</v>
       </c>
@@ -2467,12 +2417,8 @@
       <c r="J13">
         <v>60</v>
       </c>
-      <c r="L13">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63347083087802003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>237</v>
       </c>
@@ -2503,12 +2449,8 @@
       <c r="J14">
         <v>45</v>
       </c>
-      <c r="L14">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.43530701754385964</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>193</v>
       </c>
@@ -2539,12 +2481,8 @@
       <c r="J15">
         <v>55</v>
       </c>
-      <c r="L15">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49438637243515293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>190</v>
       </c>
@@ -2575,12 +2513,8 @@
       <c r="J16">
         <v>58</v>
       </c>
-      <c r="L16">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49492979719188768</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>192</v>
       </c>
@@ -2611,12 +2545,8 @@
       <c r="J17">
         <v>56</v>
       </c>
-      <c r="L17">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49922299922299923</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>239</v>
       </c>
@@ -2647,12 +2577,8 @@
       <c r="J18">
         <v>49</v>
       </c>
-      <c r="L18">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.47014523937600861</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>184</v>
       </c>
@@ -2683,12 +2609,8 @@
       <c r="J19">
         <v>53</v>
       </c>
-      <c r="L19">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50319744204636296</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>187</v>
       </c>
@@ -2719,12 +2641,8 @@
       <c r="J20">
         <v>49</v>
       </c>
-      <c r="L20">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.43233674272226591</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2755,12 +2673,8 @@
       <c r="J21">
         <v>50</v>
       </c>
-      <c r="L21">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49342481417953116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
@@ -2791,12 +2705,8 @@
       <c r="J22">
         <v>32</v>
       </c>
-      <c r="L22">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62788778877887785</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>195</v>
       </c>
@@ -2827,12 +2737,8 @@
       <c r="J23">
         <v>55</v>
       </c>
-      <c r="L23">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5422562141491396</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>236</v>
       </c>
@@ -2863,12 +2769,8 @@
       <c r="J24">
         <v>58</v>
       </c>
-      <c r="L24">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52551724137931033</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>232</v>
       </c>
@@ -2899,12 +2801,8 @@
       <c r="J25">
         <v>37</v>
       </c>
-      <c r="L25">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49554896142433236</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>213</v>
       </c>
@@ -2935,12 +2833,8 @@
       <c r="J26">
         <v>58</v>
       </c>
-      <c r="L26">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.43939393939393939</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>196</v>
       </c>
@@ -2971,12 +2865,8 @@
       <c r="J27">
         <v>51</v>
       </c>
-      <c r="L27">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49885145482388976</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
@@ -3007,12 +2897,8 @@
       <c r="J28">
         <v>28</v>
       </c>
-      <c r="L28">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58090614886731395</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>241</v>
       </c>
@@ -3043,12 +2929,8 @@
       <c r="J29">
         <v>47</v>
       </c>
-      <c r="L29">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50449497620306716</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>240</v>
       </c>
@@ -3079,12 +2961,8 @@
       <c r="J30">
         <v>46</v>
       </c>
-      <c r="L30">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51449853684490554</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>201</v>
       </c>
@@ -3115,12 +2993,8 @@
       <c r="J31">
         <v>52</v>
       </c>
-      <c r="L31">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.46082089552238809</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>235</v>
       </c>
@@ -3151,12 +3025,8 @@
       <c r="J32">
         <v>54</v>
       </c>
-      <c r="L32">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50900027693159788</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>199</v>
       </c>
@@ -3187,12 +3057,8 @@
       <c r="J33">
         <v>51</v>
       </c>
-      <c r="L33">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.4943524096385542</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>231</v>
       </c>
@@ -3223,12 +3089,8 @@
       <c r="J34">
         <v>45</v>
       </c>
-      <c r="L34">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5048632218844985</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>194</v>
       </c>
@@ -3259,12 +3121,8 @@
       <c r="J35">
         <v>54</v>
       </c>
-      <c r="L35">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.44286263947672183</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>200</v>
       </c>
@@ -3295,12 +3153,8 @@
       <c r="J36">
         <v>56</v>
       </c>
-      <c r="L36">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50149925037481258</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>98</v>
       </c>
@@ -3331,12 +3185,8 @@
       <c r="J37">
         <v>28</v>
       </c>
-      <c r="L37">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6429765886287625</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>198</v>
       </c>
@@ -3367,12 +3217,8 @@
       <c r="J38">
         <v>50</v>
       </c>
-      <c r="L38">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48299319727891155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>182</v>
       </c>
@@ -3403,12 +3249,8 @@
       <c r="J39">
         <v>58</v>
       </c>
-      <c r="L39">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52652733118971062</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>228</v>
       </c>
@@ -3439,12 +3281,8 @@
       <c r="J40">
         <v>44</v>
       </c>
-      <c r="L40">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48554533508541392</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>197</v>
       </c>
@@ -3475,12 +3313,8 @@
       <c r="J41">
         <v>57</v>
       </c>
-      <c r="L41">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48554033485540332</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>238</v>
       </c>
@@ -3511,12 +3345,8 @@
       <c r="J42">
         <v>42</v>
       </c>
-      <c r="L42">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5383777898747959</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -3547,12 +3377,8 @@
       <c r="J43">
         <v>43</v>
       </c>
-      <c r="L43">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52214285714285713</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>209</v>
       </c>
@@ -3583,12 +3409,8 @@
       <c r="J44">
         <v>59</v>
       </c>
-      <c r="L44">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54998141954663693</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>181</v>
       </c>
@@ -3619,12 +3441,8 @@
       <c r="J45">
         <v>47</v>
       </c>
-      <c r="L45">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.46231358323256749</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>230</v>
       </c>
@@ -3655,12 +3473,8 @@
       <c r="J46">
         <v>54</v>
       </c>
-      <c r="L46">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50344827586206897</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>170</v>
       </c>
@@ -3691,12 +3505,8 @@
       <c r="J47">
         <v>54</v>
       </c>
-      <c r="L47">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52045550400674823</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>229</v>
       </c>
@@ -3727,12 +3537,8 @@
       <c r="J48">
         <v>50</v>
       </c>
-      <c r="L48">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49576547231270357</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>165</v>
       </c>
@@ -3763,12 +3569,8 @@
       <c r="J49">
         <v>58</v>
       </c>
-      <c r="L49">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51768766177739434</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>223</v>
       </c>
@@ -3799,12 +3601,8 @@
       <c r="J50">
         <v>52</v>
       </c>
-      <c r="L50">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.43758480325644505</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>168</v>
       </c>
@@ -3835,12 +3633,8 @@
       <c r="J51">
         <v>63</v>
       </c>
-      <c r="L51">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54065559812686248</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>185</v>
       </c>
@@ -3871,12 +3665,8 @@
       <c r="J52">
         <v>51</v>
       </c>
-      <c r="L52">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.47471127041019512</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>173</v>
       </c>
@@ -3907,12 +3697,8 @@
       <c r="J53">
         <v>56</v>
       </c>
-      <c r="L53">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50684931506849318</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>226</v>
       </c>
@@ -3943,12 +3729,8 @@
       <c r="J54">
         <v>55</v>
       </c>
-      <c r="L54">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49282615949282615</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>203</v>
       </c>
@@ -3979,12 +3761,8 @@
       <c r="J55">
         <v>50</v>
       </c>
-      <c r="L55">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5046347793845013</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>150</v>
       </c>
@@ -4015,12 +3793,8 @@
       <c r="J56">
         <v>56</v>
       </c>
-      <c r="L56">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.55916125811283079</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>163</v>
       </c>
@@ -4051,12 +3825,8 @@
       <c r="J57">
         <v>61</v>
       </c>
-      <c r="L57">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52364273204903677</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>126</v>
       </c>
@@ -4087,12 +3857,8 @@
       <c r="J58">
         <v>44</v>
       </c>
-      <c r="L58">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.64398280802292263</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>227</v>
       </c>
@@ -4123,12 +3889,8 @@
       <c r="J59">
         <v>57</v>
       </c>
-      <c r="L59">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5175033025099075</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>130</v>
       </c>
@@ -4159,12 +3921,8 @@
       <c r="J60">
         <v>46</v>
       </c>
-      <c r="L60">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.56215469613259672</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>159</v>
       </c>
@@ -4195,12 +3953,8 @@
       <c r="J61">
         <v>51</v>
       </c>
-      <c r="L61">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.60621288259479211</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>219</v>
       </c>
@@ -4231,12 +3985,8 @@
       <c r="J62">
         <v>56</v>
       </c>
-      <c r="L62">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52427523576667834</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>225</v>
       </c>
@@ -4267,12 +4017,8 @@
       <c r="J63">
         <v>56</v>
       </c>
-      <c r="L63">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50419041233657391</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>202</v>
       </c>
@@ -4303,12 +4049,8 @@
       <c r="J64">
         <v>56</v>
       </c>
-      <c r="L64">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.4879047264607369</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>122</v>
       </c>
@@ -4339,12 +4081,8 @@
       <c r="J65">
         <v>35</v>
       </c>
-      <c r="L65">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6758922068463219</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>112</v>
       </c>
@@ -4375,12 +4113,8 @@
       <c r="J66">
         <v>27</v>
       </c>
-      <c r="L66">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.61085271317829459</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>221</v>
       </c>
@@ -4411,12 +4145,8 @@
       <c r="J67">
         <v>62</v>
       </c>
-      <c r="L67">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53537087912087911</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>224</v>
       </c>
@@ -4447,12 +4177,8 @@
       <c r="J68">
         <v>50</v>
       </c>
-      <c r="L68">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.59185733512785998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>137</v>
       </c>
@@ -4483,12 +4209,8 @@
       <c r="J69">
         <v>52</v>
       </c>
-      <c r="L69">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5711775043936731</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>220</v>
       </c>
@@ -4519,12 +4241,8 @@
       <c r="J70">
         <v>46</v>
       </c>
-      <c r="L70">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.4829030006978367</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>217</v>
       </c>
@@ -4555,12 +4273,8 @@
       <c r="J71">
         <v>66</v>
       </c>
-      <c r="L71">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49929873772791022</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>116</v>
       </c>
@@ -4591,12 +4305,8 @@
       <c r="J72">
         <v>31</v>
       </c>
-      <c r="L72">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58716265499635301</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>113</v>
       </c>
@@ -4627,12 +4337,8 @@
       <c r="J73">
         <v>27</v>
       </c>
-      <c r="L73">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.66718506998444793</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>138</v>
       </c>
@@ -4663,12 +4369,8 @@
       <c r="J74">
         <v>58</v>
       </c>
-      <c r="L74">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.66919929865575689</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>216</v>
       </c>
@@ -4699,12 +4401,8 @@
       <c r="J75">
         <v>79</v>
       </c>
-      <c r="L75">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50070175438596487</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>211</v>
       </c>
@@ -4735,12 +4433,8 @@
       <c r="J76">
         <v>58</v>
       </c>
-      <c r="L76">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51656352384419368</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>222</v>
       </c>
@@ -4771,12 +4465,8 @@
       <c r="J77">
         <v>54</v>
       </c>
-      <c r="L77">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52301397886123424</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>90</v>
       </c>
@@ -4807,12 +4497,8 @@
       <c r="J78">
         <v>27</v>
       </c>
-      <c r="L78">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.65285451197053412</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>215</v>
       </c>
@@ -4843,12 +4529,8 @@
       <c r="J79">
         <v>56</v>
       </c>
-      <c r="L79">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53743409490333915</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>204</v>
       </c>
@@ -4879,12 +4561,8 @@
       <c r="J80">
         <v>56</v>
       </c>
-      <c r="L80">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.49759526452090269</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>218</v>
       </c>
@@ -4915,12 +4593,8 @@
       <c r="J81">
         <v>56</v>
       </c>
-      <c r="L81">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51661420076949982</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>212</v>
       </c>
@@ -4951,12 +4625,8 @@
       <c r="J82">
         <v>47</v>
       </c>
-      <c r="L82">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52934782608695652</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>147</v>
       </c>
@@ -4987,12 +4657,8 @@
       <c r="J83">
         <v>56</v>
       </c>
-      <c r="L83">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.59140341791817708</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>208</v>
       </c>
@@ -5023,12 +4689,8 @@
       <c r="J84">
         <v>60</v>
       </c>
-      <c r="L84">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.46440306681270538</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>183</v>
       </c>
@@ -5059,12 +4721,8 @@
       <c r="J85">
         <v>51</v>
       </c>
-      <c r="L85">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.55813953488372092</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>174</v>
       </c>
@@ -5095,12 +4753,8 @@
       <c r="J86">
         <v>67</v>
       </c>
-      <c r="L86">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53316749585406298</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>210</v>
       </c>
@@ -5131,12 +4785,8 @@
       <c r="J87">
         <v>60</v>
       </c>
-      <c r="L87">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54624908958485074</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>172</v>
       </c>
@@ -5167,12 +4817,8 @@
       <c r="J88">
         <v>57</v>
       </c>
-      <c r="L88">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.47891440501043842</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>139</v>
       </c>
@@ -5203,12 +4849,8 @@
       <c r="J89">
         <v>51</v>
       </c>
-      <c r="L89">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.56130156885531668</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>177</v>
       </c>
@@ -5239,12 +4881,8 @@
       <c r="J90">
         <v>51</v>
       </c>
-      <c r="L90">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.56965688300950801</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>142</v>
       </c>
@@ -5275,12 +4913,8 @@
       <c r="J91">
         <v>50</v>
       </c>
-      <c r="L91">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57861635220125784</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>205</v>
       </c>
@@ -5311,12 +4945,8 @@
       <c r="J92">
         <v>58</v>
       </c>
-      <c r="L92">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.47605011053795138</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>141</v>
       </c>
@@ -5347,12 +4977,8 @@
       <c r="J93">
         <v>47</v>
       </c>
-      <c r="L93">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52761795166858461</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>140</v>
       </c>
@@ -5383,12 +5009,8 @@
       <c r="J94">
         <v>59</v>
       </c>
-      <c r="L94">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5597920277296361</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>175</v>
       </c>
@@ -5419,12 +5041,8 @@
       <c r="J95">
         <v>57</v>
       </c>
-      <c r="L95">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57166528583264287</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>207</v>
       </c>
@@ -5455,12 +5073,8 @@
       <c r="J96">
         <v>55</v>
       </c>
-      <c r="L96">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54215542521994131</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>214</v>
       </c>
@@ -5491,12 +5105,8 @@
       <c r="J97">
         <v>46</v>
       </c>
-      <c r="L97">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52709359605911332</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>178</v>
       </c>
@@ -5527,12 +5137,8 @@
       <c r="J98">
         <v>46</v>
       </c>
-      <c r="L98">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57131079967023912</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>171</v>
       </c>
@@ -5563,12 +5169,8 @@
       <c r="J99">
         <v>59</v>
       </c>
-      <c r="L99">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58469259723964873</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>206</v>
       </c>
@@ -5599,12 +5201,8 @@
       <c r="J100">
         <v>55</v>
       </c>
-      <c r="L100">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50367917586460631</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>179</v>
       </c>
@@ -5635,12 +5233,8 @@
       <c r="J101">
         <v>49</v>
       </c>
-      <c r="L101">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48226661231145534</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>117</v>
       </c>
@@ -5671,12 +5265,8 @@
       <c r="J102">
         <v>29</v>
       </c>
-      <c r="L102">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.70626822157434399</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>118</v>
       </c>
@@ -5707,12 +5297,8 @@
       <c r="J103">
         <v>32</v>
       </c>
-      <c r="L103">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.61163636363636364</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>134</v>
       </c>
@@ -5743,12 +5329,8 @@
       <c r="J104">
         <v>52</v>
       </c>
-      <c r="L104">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51297814207650272</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>167</v>
       </c>
@@ -5779,12 +5361,8 @@
       <c r="J105">
         <v>62</v>
       </c>
-      <c r="L105">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58244111349036398</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>102</v>
       </c>
@@ -5815,12 +5393,8 @@
       <c r="J106">
         <v>30</v>
       </c>
-      <c r="L106">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>2.262295081967213</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>162</v>
       </c>
@@ -5851,12 +5425,8 @@
       <c r="J107">
         <v>56</v>
       </c>
-      <c r="L107">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5742832319721981</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>51</v>
       </c>
@@ -5887,12 +5457,8 @@
       <c r="J108">
         <v>30</v>
       </c>
-      <c r="L108">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6033376123234917</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>176</v>
       </c>
@@ -5923,12 +5489,8 @@
       <c r="J109">
         <v>57</v>
       </c>
-      <c r="L109">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57509309060819203</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>160</v>
       </c>
@@ -5959,12 +5521,8 @@
       <c r="J110">
         <v>67</v>
       </c>
-      <c r="L110">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.56773618538324422</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>166</v>
       </c>
@@ -5995,12 +5553,8 @@
       <c r="J111">
         <v>57</v>
       </c>
-      <c r="L111">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53879310344827591</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>169</v>
       </c>
@@ -6031,12 +5585,8 @@
       <c r="J112">
         <v>67</v>
       </c>
-      <c r="L112">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53836371343789746</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>161</v>
       </c>
@@ -6067,12 +5617,8 @@
       <c r="J113">
         <v>61</v>
       </c>
-      <c r="L113">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51339481774264384</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>129</v>
       </c>
@@ -6103,12 +5649,8 @@
       <c r="J114">
         <v>51</v>
       </c>
-      <c r="L114">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>88</v>
       </c>
@@ -6139,12 +5681,8 @@
       <c r="J115">
         <v>35</v>
       </c>
-      <c r="L115">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.73929236499068907</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
@@ -6175,12 +5713,8 @@
       <c r="J116">
         <v>47</v>
       </c>
-      <c r="L116">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53402646502835538</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>154</v>
       </c>
@@ -6211,12 +5745,8 @@
       <c r="J117">
         <v>57</v>
       </c>
-      <c r="L117">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53058252427184471</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>123</v>
       </c>
@@ -6247,12 +5777,8 @@
       <c r="J118">
         <v>46</v>
       </c>
-      <c r="L118">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.52536231884057971</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>132</v>
       </c>
@@ -6283,12 +5809,8 @@
       <c r="J119">
         <v>47</v>
       </c>
-      <c r="L119">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5339739190116678</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>152</v>
       </c>
@@ -6319,12 +5841,8 @@
       <c r="J120">
         <v>59</v>
       </c>
-      <c r="L120">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58543689320388348</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -6355,12 +5873,8 @@
       <c r="J121">
         <v>33</v>
       </c>
-      <c r="L121">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51237263464337701</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>128</v>
       </c>
@@ -6391,12 +5905,8 @@
       <c r="J122">
         <v>40</v>
       </c>
-      <c r="L122">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.56642857142857139</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>135</v>
       </c>
@@ -6427,12 +5937,8 @@
       <c r="J123">
         <v>52</v>
       </c>
-      <c r="L123">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63251817580964975</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>149</v>
       </c>
@@ -6463,12 +5969,8 @@
       <c r="J124">
         <v>55</v>
       </c>
-      <c r="L124">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.55366098294884658</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>155</v>
       </c>
@@ -6499,12 +6001,8 @@
       <c r="J125">
         <v>54</v>
       </c>
-      <c r="L125">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54528122020972358</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
@@ -6535,12 +6033,8 @@
       <c r="J126">
         <v>44</v>
       </c>
-      <c r="L126">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.43768115942028984</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>156</v>
       </c>
@@ -6571,12 +6065,8 @@
       <c r="J127">
         <v>64</v>
       </c>
-      <c r="L127">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57054041128646582</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>119</v>
       </c>
@@ -6607,12 +6097,8 @@
       <c r="J128">
         <v>33</v>
       </c>
-      <c r="L128">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5905454545454546</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>111</v>
       </c>
@@ -6643,12 +6129,8 @@
       <c r="J129">
         <v>33</v>
       </c>
-      <c r="L129">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62994569433669512</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>153</v>
       </c>
@@ -6679,12 +6161,8 @@
       <c r="J130">
         <v>59</v>
       </c>
-      <c r="L130">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.60490196078431369</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>101</v>
       </c>
@@ -6715,12 +6193,8 @@
       <c r="J131">
         <v>29</v>
       </c>
-      <c r="L131">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6389337641357028</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>121</v>
       </c>
@@ -6751,12 +6225,8 @@
       <c r="J132">
         <v>31</v>
       </c>
-      <c r="L132">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57121986851716577</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>133</v>
       </c>
@@ -6787,12 +6257,8 @@
       <c r="J133">
         <v>55</v>
       </c>
-      <c r="L133">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.59766963673749141</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>78</v>
       </c>
@@ -6823,12 +6289,8 @@
       <c r="J134">
         <v>33</v>
       </c>
-      <c r="L134">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6044921875</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>86</v>
       </c>
@@ -6859,12 +6321,8 @@
       <c r="J135">
         <v>32</v>
       </c>
-      <c r="L135">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62476547842401498</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>180</v>
       </c>
@@ -6895,12 +6353,8 @@
       <c r="J136">
         <v>50</v>
       </c>
-      <c r="L136">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58711507293354948</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>103</v>
       </c>
@@ -6931,12 +6385,8 @@
       <c r="J137">
         <v>24</v>
       </c>
-      <c r="L137">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.61755233494363926</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>146</v>
       </c>
@@ -6967,12 +6417,8 @@
       <c r="J138">
         <v>54</v>
       </c>
-      <c r="L138">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63413304252998914</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>95</v>
       </c>
@@ -7003,12 +6449,8 @@
       <c r="J139">
         <v>32</v>
       </c>
-      <c r="L139">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.55191256830601088</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>145</v>
       </c>
@@ -7039,12 +6481,8 @@
       <c r="J140">
         <v>57</v>
       </c>
-      <c r="L140">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6321967579653438</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>125</v>
       </c>
@@ -7075,12 +6513,8 @@
       <c r="J141">
         <v>45</v>
       </c>
-      <c r="L141">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.448150833937636</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>115</v>
       </c>
@@ -7111,12 +6545,8 @@
       <c r="J142">
         <v>32</v>
       </c>
-      <c r="L142">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5527086383601757</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>93</v>
       </c>
@@ -7147,12 +6577,8 @@
       <c r="J143">
         <v>30</v>
       </c>
-      <c r="L143">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.74152153987167735</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>104</v>
       </c>
@@ -7183,12 +6609,8 @@
       <c r="J144">
         <v>31</v>
       </c>
-      <c r="L144">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58686949559647716</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>107</v>
       </c>
@@ -7219,12 +6641,8 @@
       <c r="J145">
         <v>30</v>
       </c>
-      <c r="L145">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.65939204988308653</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>114</v>
       </c>
@@ -7255,12 +6673,8 @@
       <c r="J146">
         <v>34</v>
       </c>
-      <c r="L146">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.60575427682737171</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>108</v>
       </c>
@@ -7291,12 +6705,8 @@
       <c r="J147">
         <v>30</v>
       </c>
-      <c r="L147">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.2941634241245137</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>144</v>
       </c>
@@ -7327,12 +6737,8 @@
       <c r="J148">
         <v>53</v>
       </c>
-      <c r="L148">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48379761227970436</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>97</v>
       </c>
@@ -7363,12 +6769,8 @@
       <c r="J149">
         <v>31</v>
       </c>
-      <c r="L149">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.66552315608919388</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>143</v>
       </c>
@@ -7399,12 +6801,8 @@
       <c r="J150">
         <v>47</v>
       </c>
-      <c r="L150">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.58494868871151651</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>109</v>
       </c>
@@ -7435,12 +6833,8 @@
       <c r="J151">
         <v>31</v>
       </c>
-      <c r="L151">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.60852713178294571</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>105</v>
       </c>
@@ -7471,12 +6865,8 @@
       <c r="J152">
         <v>28</v>
       </c>
-      <c r="L152">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5591054313099042</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>110</v>
       </c>
@@ -7507,12 +6897,8 @@
       <c r="J153">
         <v>38</v>
       </c>
-      <c r="L153">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53374709076803728</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>106</v>
       </c>
@@ -7543,12 +6929,8 @@
       <c r="J154">
         <v>28</v>
       </c>
-      <c r="L154">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.60637450199203191</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>85</v>
       </c>
@@ -7579,12 +6961,8 @@
       <c r="J155">
         <v>27</v>
       </c>
-      <c r="L155">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.59624413145539901</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>89</v>
       </c>
@@ -7615,12 +6993,8 @@
       <c r="J156">
         <v>28</v>
       </c>
-      <c r="L156">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.71244239631336403</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>79</v>
       </c>
@@ -7651,12 +7025,8 @@
       <c r="J157">
         <v>28</v>
       </c>
-      <c r="L157">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5812379110251451</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>91</v>
       </c>
@@ -7687,12 +7057,8 @@
       <c r="J158">
         <v>29</v>
       </c>
-      <c r="L158">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.61376146788990826</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>92</v>
       </c>
@@ -7723,12 +7089,8 @@
       <c r="J159">
         <v>29</v>
       </c>
-      <c r="L159">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.69287696577243296</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>76</v>
       </c>
@@ -7759,12 +7121,8 @@
       <c r="J160">
         <v>29</v>
       </c>
-      <c r="L160">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6181998021760633</v>
-      </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>17</v>
       </c>
@@ -7795,12 +7153,8 @@
       <c r="J161">
         <v>29</v>
       </c>
-      <c r="L161">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.84276729559748431</v>
-      </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>82</v>
       </c>
@@ -7831,12 +7185,8 @@
       <c r="J162">
         <v>27</v>
       </c>
-      <c r="L162">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.56792452830188678</v>
-      </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>96</v>
       </c>
@@ -7867,12 +7217,8 @@
       <c r="J163">
         <v>34</v>
       </c>
-      <c r="L163">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.65209471766848814</v>
-      </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>94</v>
       </c>
@@ -7903,12 +7249,8 @@
       <c r="J164">
         <v>30</v>
       </c>
-      <c r="L164">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62362637362637363</v>
-      </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>31</v>
       </c>
@@ -7939,12 +7281,8 @@
       <c r="J165">
         <v>27</v>
       </c>
-      <c r="L165">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.93991416309012876</v>
-      </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>87</v>
       </c>
@@ -7975,12 +7313,8 @@
       <c r="J166">
         <v>33</v>
       </c>
-      <c r="L166">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.64738805970149249</v>
-      </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>83</v>
       </c>
@@ -8011,12 +7345,8 @@
       <c r="J167">
         <v>29</v>
       </c>
-      <c r="L167">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.48496240601503759</v>
-      </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>84</v>
       </c>
@@ -8047,12 +7377,8 @@
       <c r="J168">
         <v>28</v>
       </c>
-      <c r="L168">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.61806208842897459</v>
-      </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>80</v>
       </c>
@@ -8083,12 +7409,8 @@
       <c r="J169">
         <v>29</v>
       </c>
-      <c r="L169">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5428296438883542</v>
-      </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>71</v>
       </c>
@@ -8119,12 +7441,8 @@
       <c r="J170">
         <v>31</v>
       </c>
-      <c r="L170">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5930372148859544</v>
-      </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>81</v>
       </c>
@@ -8155,12 +7473,8 @@
       <c r="J171">
         <v>29</v>
       </c>
-      <c r="L171">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.69856459330143539</v>
-      </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>77</v>
       </c>
@@ -8191,12 +7505,8 @@
       <c r="J172">
         <v>35</v>
       </c>
-      <c r="L172">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57976653696498059</v>
-      </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>64</v>
       </c>
@@ -8227,12 +7537,8 @@
       <c r="J173">
         <v>27</v>
       </c>
-      <c r="L173">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53284671532846717</v>
-      </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>60</v>
       </c>
@@ -8263,12 +7569,8 @@
       <c r="J174">
         <v>26</v>
       </c>
-      <c r="L174">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53056234718826401</v>
-      </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>65</v>
       </c>
@@ -8299,12 +7601,8 @@
       <c r="J175">
         <v>28</v>
       </c>
-      <c r="L175">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.45344619105199518</v>
-      </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>73</v>
       </c>
@@ -8335,12 +7633,8 @@
       <c r="J176">
         <v>24</v>
       </c>
-      <c r="L176">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51079136690647486</v>
-      </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>25</v>
       </c>
@@ -8371,12 +7665,8 @@
       <c r="J177">
         <v>35</v>
       </c>
-      <c r="L177">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.70250368188512513</v>
-      </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>27</v>
       </c>
@@ -8407,12 +7697,8 @@
       <c r="J178">
         <v>28</v>
       </c>
-      <c r="L178">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.72423802612481858</v>
-      </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>50</v>
       </c>
@@ -8443,12 +7729,8 @@
       <c r="J179">
         <v>35</v>
       </c>
-      <c r="L179">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.70375161707632605</v>
-      </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>32</v>
       </c>
@@ -8479,12 +7761,8 @@
       <c r="J180">
         <v>23</v>
       </c>
-      <c r="L180">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.81054131054131051</v>
-      </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>29</v>
       </c>
@@ -8515,12 +7793,8 @@
       <c r="J181">
         <v>25</v>
       </c>
-      <c r="L181">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.74529667149059331</v>
-      </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>59</v>
       </c>
@@ -8551,12 +7825,8 @@
       <c r="J182">
         <v>33</v>
       </c>
-      <c r="L182">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.60643564356435642</v>
-      </c>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>44</v>
       </c>
@@ -8587,12 +7857,8 @@
       <c r="J183">
         <v>33</v>
       </c>
-      <c r="L183">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.71680216802168017</v>
-      </c>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>44</v>
       </c>
@@ -8623,12 +7889,8 @@
       <c r="J184">
         <v>33</v>
       </c>
-      <c r="L184">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.71680216802168017</v>
-      </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>23</v>
       </c>
@@ -8659,12 +7921,8 @@
       <c r="J185">
         <v>31</v>
       </c>
-      <c r="L185">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.95956454121306378</v>
-      </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>30</v>
       </c>
@@ -8695,12 +7953,8 @@
       <c r="J186">
         <v>32</v>
       </c>
-      <c r="L186">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.7496402877697842</v>
-      </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>47</v>
       </c>
@@ -8731,12 +7985,8 @@
       <c r="J187">
         <v>28</v>
       </c>
-      <c r="L187">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6511936339522546</v>
-      </c>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>53</v>
       </c>
@@ -8767,12 +8017,8 @@
       <c r="J188">
         <v>29</v>
       </c>
-      <c r="L188">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63775510204081631</v>
-      </c>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>62</v>
       </c>
@@ -8803,12 +8049,8 @@
       <c r="J189">
         <v>29</v>
       </c>
-      <c r="L189">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63048780487804879</v>
-      </c>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>49</v>
       </c>
@@ -8839,12 +8081,8 @@
       <c r="J190">
         <v>31</v>
       </c>
-      <c r="L190">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.61942257217847774</v>
-      </c>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>40</v>
       </c>
@@ -8875,12 +8113,8 @@
       <c r="J191">
         <v>28</v>
       </c>
-      <c r="L191">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63114754098360659</v>
-      </c>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>66</v>
       </c>
@@ -8911,12 +8145,8 @@
       <c r="J192">
         <v>25</v>
       </c>
-      <c r="L192">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54050785973397819</v>
-      </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>28</v>
       </c>
@@ -8947,12 +8177,8 @@
       <c r="J193">
         <v>30</v>
       </c>
-      <c r="L193">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.7858176555716353</v>
-      </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>55</v>
       </c>
@@ -8983,12 +8209,8 @@
       <c r="J194">
         <v>26</v>
       </c>
-      <c r="L194">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5462610899873257</v>
-      </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>72</v>
       </c>
@@ -9019,12 +8241,8 @@
       <c r="J195">
         <v>29</v>
       </c>
-      <c r="L195">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5311750599520384</v>
-      </c>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>61</v>
       </c>
@@ -9055,12 +8273,8 @@
       <c r="J196">
         <v>28</v>
       </c>
-      <c r="L196">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.67245657568238215</v>
-      </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>41</v>
       </c>
@@ -9091,12 +8305,8 @@
       <c r="J197">
         <v>29</v>
       </c>
-      <c r="L197">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63437926330150063</v>
-      </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>74</v>
       </c>
@@ -9127,12 +8337,8 @@
       <c r="J198">
         <v>28</v>
       </c>
-      <c r="L198">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.50765606595995294</v>
-      </c>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>70</v>
       </c>
@@ -9163,12 +8369,8 @@
       <c r="J199">
         <v>31</v>
       </c>
-      <c r="L199">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.55942376950780315</v>
-      </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>68</v>
       </c>
@@ -9199,12 +8401,8 @@
       <c r="J200">
         <v>29</v>
       </c>
-      <c r="L200">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.64776839565741862</v>
-      </c>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>67</v>
       </c>
@@ -9235,12 +8433,8 @@
       <c r="J201">
         <v>28</v>
       </c>
-      <c r="L201">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.66827503015681544</v>
-      </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>63</v>
       </c>
@@ -9271,12 +8465,8 @@
       <c r="J202">
         <v>26</v>
       </c>
-      <c r="L202">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.0916870415647921</v>
-      </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>75</v>
       </c>
@@ -9307,12 +8497,8 @@
       <c r="J203">
         <v>31</v>
       </c>
-      <c r="L203">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.63540445486518171</v>
-      </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>35</v>
       </c>
@@ -9343,12 +8529,8 @@
       <c r="J204">
         <v>29</v>
       </c>
-      <c r="L204">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.80198019801980203</v>
-      </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>39</v>
       </c>
@@ -9379,12 +8561,8 @@
       <c r="J205">
         <v>31</v>
       </c>
-      <c r="L205">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.70491803278688525</v>
-      </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>52</v>
       </c>
@@ -9415,12 +8593,8 @@
       <c r="J206">
         <v>27</v>
       </c>
-      <c r="L206">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.64240102171136659</v>
-      </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>48</v>
       </c>
@@ -9451,12 +8625,8 @@
       <c r="J207">
         <v>32</v>
       </c>
-      <c r="L207">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62668463611859837</v>
-      </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>26</v>
       </c>
@@ -9487,12 +8657,8 @@
       <c r="J208">
         <v>32</v>
       </c>
-      <c r="L208">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.82959641255605376</v>
-      </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>54</v>
       </c>
@@ -9523,12 +8689,8 @@
       <c r="J209">
         <v>24</v>
       </c>
-      <c r="L209">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.5592356687898089</v>
-      </c>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>69</v>
       </c>
@@ -9559,12 +8721,8 @@
       <c r="J210">
         <v>25</v>
       </c>
-      <c r="L210">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.55595667870036103</v>
-      </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>56</v>
       </c>
@@ -9595,12 +8753,8 @@
       <c r="J211">
         <v>30</v>
       </c>
-      <c r="L211">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.54522613065326631</v>
-      </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>24</v>
       </c>
@@ -9631,12 +8785,8 @@
       <c r="J212">
         <v>36</v>
       </c>
-      <c r="L212">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.75642965204236001</v>
-      </c>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>57</v>
       </c>
@@ -9667,12 +8817,8 @@
       <c r="J213">
         <v>27</v>
       </c>
-      <c r="L213">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.53316645807259078</v>
-      </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>58</v>
       </c>
@@ -9703,12 +8849,8 @@
       <c r="J214">
         <v>32</v>
       </c>
-      <c r="L214">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.723114956736712</v>
-      </c>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>46</v>
       </c>
@@ -9739,12 +8881,8 @@
       <c r="J215">
         <v>24</v>
       </c>
-      <c r="L215">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.78734858681022879</v>
-      </c>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>33</v>
       </c>
@@ -9775,12 +8913,8 @@
       <c r="J216">
         <v>28</v>
       </c>
-      <c r="L216">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.79290780141843975</v>
-      </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>42</v>
       </c>
@@ -9811,12 +8945,8 @@
       <c r="J217">
         <v>32</v>
       </c>
-      <c r="L217">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.57394843962008146</v>
-      </c>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>37</v>
       </c>
@@ -9847,12 +8977,8 @@
       <c r="J218">
         <v>26</v>
       </c>
-      <c r="L218">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.81206171107994385</v>
-      </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>43</v>
       </c>
@@ -9883,12 +9009,8 @@
       <c r="J219">
         <v>34</v>
       </c>
-      <c r="L219">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.80732700135685209</v>
-      </c>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>38</v>
       </c>
@@ -9919,12 +9041,8 @@
       <c r="J220">
         <v>32</v>
       </c>
-      <c r="L220">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.6333789329685362</v>
-      </c>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>34</v>
       </c>
@@ -9955,12 +9073,8 @@
       <c r="J221">
         <v>30</v>
       </c>
-      <c r="L221">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.62127659574468086</v>
-      </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>45</v>
       </c>
@@ -9991,12 +9105,8 @@
       <c r="J222">
         <v>29</v>
       </c>
-      <c r="L222">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.51413189771197843</v>
-      </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>21</v>
       </c>
@@ -10027,12 +9137,8 @@
       <c r="J223">
         <v>34</v>
       </c>
-      <c r="L223">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.84046692607003892</v>
-      </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>22</v>
       </c>
@@ -10063,12 +9169,8 @@
       <c r="J224">
         <v>34</v>
       </c>
-      <c r="L224">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.74517374517374513</v>
-      </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>18</v>
       </c>
@@ -10099,12 +9201,8 @@
       <c r="J225">
         <v>25</v>
       </c>
-      <c r="L225">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.0331950207468881</v>
-      </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>16</v>
       </c>
@@ -10135,12 +9233,8 @@
       <c r="J226">
         <v>23</v>
       </c>
-      <c r="L226">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.77204301075268822</v>
-      </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>19</v>
       </c>
@@ -10171,12 +9265,8 @@
       <c r="J227">
         <v>27</v>
       </c>
-      <c r="L227">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.81927710843373491</v>
-      </c>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>15</v>
       </c>
@@ -10207,12 +9297,8 @@
       <c r="J228">
         <v>27</v>
       </c>
-      <c r="L228">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.76430205949656749</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>20</v>
       </c>
@@ -10243,12 +9329,8 @@
       <c r="J229">
         <v>26</v>
       </c>
-      <c r="L229">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>0.72868217054263562</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>14</v>
       </c>
@@ -10279,12 +9361,8 @@
       <c r="J230">
         <v>18</v>
       </c>
-      <c r="L230">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>3.2530120481927711</v>
-      </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>12</v>
       </c>
@@ -10315,12 +9393,8 @@
       <c r="J231">
         <v>21</v>
       </c>
-      <c r="L231">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.5769230769230769</v>
-      </c>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>13</v>
       </c>
@@ -10351,12 +9425,8 @@
       <c r="J232">
         <v>24</v>
       </c>
-      <c r="L232">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.6463414634146341</v>
-      </c>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>11</v>
       </c>
@@ -10387,12 +9457,8 @@
       <c r="J233">
         <v>21</v>
       </c>
-      <c r="L233">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.9189189189189189</v>
-      </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>10</v>
       </c>
@@ -10423,12 +9489,8 @@
       <c r="J234">
         <v>21</v>
       </c>
-      <c r="L234">
-        <f>+Table1[[#This Row],[Opens]]/Table1[[#This Row],[Sends]]</f>
-        <v>1.1724137931034482</v>
-      </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C236">
         <f>+SUM(C2:C234)</f>
         <v>390760</v>
@@ -10441,12 +9503,8 @@
         <f>+AVERAGE(Table1[Open Rate])</f>
         <v>0.62651802575107296</v>
       </c>
-      <c r="L236">
-        <f>+AVERAGE(L2:L234)</f>
-        <v>0.62651817224131723</v>
-      </c>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D237">
         <f>+D236/C236</f>
         <v>0.55507728529020373</v>

</xml_diff>